<commit_message>
Added bitmaps for all digits and capital letters
</commit_message>
<xml_diff>
--- a/display_lcd_vim828/bitmaps.xlsx
+++ b/display_lcd_vim828/bitmaps.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="19">
   <si>
     <t>Kod</t>
   </si>
@@ -417,10 +417,10 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C92" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C80" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1:P1048576"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomRight" activeCell="P67" sqref="P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -492,16 +492,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -535,7 +535,7 @@
       </c>
       <c r="Q2" s="2" t="str">
         <f>P2&amp;O2&amp;N2&amp;M2&amp;L2&amp;K2&amp;J2&amp;I2&amp;H2&amp;G2&amp;F2&amp;E2&amp;D2&amp;C2</f>
-        <v>00000000001111</v>
+        <v>00000000000000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -546,9 +546,51 @@
         <f t="shared" ref="B3:B66" si="0">CHAR(A3)</f>
         <v>_x0001_</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q3" s="2" t="str">
         <f t="shared" ref="Q3:Q66" si="1">P3&amp;O3&amp;N3&amp;M3&amp;L3&amp;K3&amp;J3&amp;I3&amp;H3&amp;G3&amp;F3&amp;E3&amp;D3&amp;C3</f>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -559,9 +601,51 @@
         <f t="shared" si="0"/>
         <v>_x0002_</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -572,9 +656,51 @@
         <f t="shared" si="0"/>
         <v>_x0003_</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -585,9 +711,51 @@
         <f t="shared" si="0"/>
         <v>_x0004_</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -598,9 +766,51 @@
         <f t="shared" si="0"/>
         <v>_x0005_</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -611,9 +821,51 @@
         <f t="shared" si="0"/>
         <v>_x0006_</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -624,9 +876,51 @@
         <f t="shared" si="0"/>
         <v>_x0007_</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -637,9 +931,51 @@
         <f t="shared" si="0"/>
         <v>_x0008_</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -650,9 +986,51 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">	</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -664,9 +1042,51 @@
         <v xml:space="preserve">
 </v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -677,9 +1097,51 @@
         <f t="shared" si="0"/>
         <v>_x000B_</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -690,9 +1152,51 @@
         <f t="shared" si="0"/>
         <v>_x000C_</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -703,9 +1207,51 @@
         <f t="shared" si="0"/>
         <v>_x000D_</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -716,9 +1262,51 @@
         <f t="shared" si="0"/>
         <v>_x000E_</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -729,9 +1317,51 @@
         <f t="shared" si="0"/>
         <v>_x000F_</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -742,9 +1372,51 @@
         <f t="shared" si="0"/>
         <v>_x0010_</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -755,9 +1427,51 @@
         <f t="shared" si="0"/>
         <v>_x0011_</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -768,9 +1482,51 @@
         <f t="shared" si="0"/>
         <v>_x0012_</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -781,9 +1537,51 @@
         <f t="shared" si="0"/>
         <v>_x0013_</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -794,9 +1592,51 @@
         <f t="shared" si="0"/>
         <v>_x0014_</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -807,9 +1647,51 @@
         <f t="shared" si="0"/>
         <v>_x0015_</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -820,9 +1702,51 @@
         <f t="shared" si="0"/>
         <v>_x0016_</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -833,9 +1757,51 @@
         <f t="shared" si="0"/>
         <v>_x0017_</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -846,9 +1812,51 @@
         <f t="shared" si="0"/>
         <v>_x0018_</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -859,9 +1867,51 @@
         <f t="shared" si="0"/>
         <v>_x0019_</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -872,9 +1922,51 @@
         <f t="shared" si="0"/>
         <v>_x001A_</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -885,9 +1977,51 @@
         <f t="shared" si="0"/>
         <v>_x001B_</v>
       </c>
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -898,9 +2032,51 @@
         <f t="shared" si="0"/>
         <v>_x001C_</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -911,9 +2087,51 @@
         <f t="shared" si="0"/>
         <v>_x001D_</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -924,9 +2142,51 @@
         <f t="shared" si="0"/>
         <v>_x001E_</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -937,9 +2197,51 @@
         <f t="shared" si="0"/>
         <v>_x001F_</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -1115,9 +2417,51 @@
         <f t="shared" si="0"/>
         <v>#</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -1183,9 +2527,51 @@
         <f t="shared" si="0"/>
         <v>%</v>
       </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>00101000100100</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -1196,9 +2582,51 @@
         <f t="shared" si="0"/>
         <v>&amp;</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -2254,9 +3682,51 @@
         <f t="shared" si="0"/>
         <v>:</v>
       </c>
+      <c r="C60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q60" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -2267,9 +3737,51 @@
         <f t="shared" si="0"/>
         <v>;</v>
       </c>
+      <c r="C61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q61" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11111111111111</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -2500,9 +4012,51 @@
         <f t="shared" si="0"/>
         <v>@</v>
       </c>
+      <c r="C66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q66" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>00010000111011</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -2513,9 +4067,51 @@
         <f t="shared" ref="B67:B129" si="2">CHAR(A67)</f>
         <v>A</v>
       </c>
+      <c r="C67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q67" s="2" t="str">
         <f t="shared" ref="Q67:Q129" si="3">P67&amp;O67&amp;N67&amp;M67&amp;L67&amp;K67&amp;J67&amp;I67&amp;H67&amp;G67&amp;F67&amp;E67&amp;D67&amp;C67</f>
-        <v/>
+        <v>00010001110111</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -2526,9 +4122,51 @@
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
+      <c r="C68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q68" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01010100001111</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -2539,9 +4177,51 @@
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
+      <c r="C69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P69" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q69" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000000111001</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -2552,9 +4232,51 @@
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
+      <c r="C70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P70" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q70" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000100001111</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -2565,9 +4287,51 @@
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
+      <c r="C71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q71" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001111001</v>
       </c>
     </row>
     <row r="72" spans="1:17">
@@ -2578,9 +4342,51 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
+      <c r="C72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q72" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001110001</v>
       </c>
     </row>
     <row r="73" spans="1:17">
@@ -2591,9 +4397,51 @@
         <f t="shared" si="2"/>
         <v>G</v>
       </c>
+      <c r="C73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q73" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00010000111101</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -2604,9 +4452,51 @@
         <f t="shared" si="2"/>
         <v>H</v>
       </c>
+      <c r="C74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q74" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00010001110110</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -2617,9 +4507,51 @@
         <f t="shared" si="2"/>
         <v>I</v>
       </c>
+      <c r="C75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q75" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000100001001</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -2630,9 +4562,51 @@
         <f t="shared" si="2"/>
         <v>J</v>
       </c>
+      <c r="C76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q76" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000000011110</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -2643,9 +4617,51 @@
         <f t="shared" si="2"/>
         <v>K</v>
       </c>
+      <c r="C77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q77" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10001001110000</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -2656,9 +4672,51 @@
         <f t="shared" si="2"/>
         <v>L</v>
       </c>
+      <c r="C78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P78" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q78" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000000111000</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -2669,9 +4727,51 @@
         <f t="shared" si="2"/>
         <v>M</v>
       </c>
+      <c r="C79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q79" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00001010110110</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -2682,9 +4782,51 @@
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
+      <c r="C80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q80" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000010110110</v>
       </c>
     </row>
     <row r="81" spans="1:17">
@@ -2695,9 +4837,51 @@
         <f t="shared" si="2"/>
         <v>O</v>
       </c>
+      <c r="C81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q81" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000000111111</v>
       </c>
     </row>
     <row r="82" spans="1:17">
@@ -2708,9 +4892,51 @@
         <f t="shared" si="2"/>
         <v>P</v>
       </c>
+      <c r="C82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P82" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q82" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00010000110011</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -2721,9 +4947,51 @@
         <f t="shared" si="2"/>
         <v>Q</v>
       </c>
+      <c r="C83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q83" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000000111111</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -2734,9 +5002,51 @@
         <f t="shared" si="2"/>
         <v>R</v>
       </c>
+      <c r="C84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P84" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q84" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10010001110011</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -2747,9 +5057,51 @@
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
+      <c r="C85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P85" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q85" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00010001101101</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -2760,9 +5112,51 @@
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
+      <c r="C86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P86" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q86" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000100000001</v>
       </c>
     </row>
     <row r="87" spans="1:17">
@@ -2773,9 +5167,51 @@
         <f t="shared" si="2"/>
         <v>U</v>
       </c>
+      <c r="C87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P87" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q87" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000000111110</v>
       </c>
     </row>
     <row r="88" spans="1:17">
@@ -2786,9 +5222,51 @@
         <f t="shared" si="2"/>
         <v>V</v>
       </c>
+      <c r="C88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P88" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q88" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00101000110000</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -2799,9 +5277,51 @@
         <f t="shared" si="2"/>
         <v>W</v>
       </c>
+      <c r="C89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P89" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q89" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10100000110110</v>
       </c>
     </row>
     <row r="90" spans="1:17">
@@ -2812,9 +5332,51 @@
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
+      <c r="C90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="Q90" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10101010000000</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -2825,9 +5387,51 @@
         <f t="shared" si="2"/>
         <v>Y</v>
       </c>
+      <c r="C91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P91" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q91" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01001010000000</v>
       </c>
     </row>
     <row r="92" spans="1:17">
@@ -2838,9 +5442,51 @@
         <f t="shared" si="2"/>
         <v>Z</v>
       </c>
+      <c r="C92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P92" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q92" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00101000001001</v>
       </c>
     </row>
     <row r="93" spans="1:17">

</xml_diff>